<commit_message>
cambios de nomenclatura e inclusión de calderas
</commit_message>
<xml_diff>
--- a/Catalogo.xlsx
+++ b/Catalogo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Documents\GitHub\PC_optimizacion\Tesis Luis Leon\Códigos Función min costos\Códigos finales\Capitulo_estocastico\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Documents\GitHub\Tesis_Maestria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A137F5-6698-45B1-9CB4-9786AD2BFBAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B77AB4-379A-4730-BCF4-F5DAD1C0CCB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="599" activeTab="5" xr2:uid="{27070F80-89CF-4E15-8F14-835BDE193743}"/>
+    <workbookView xWindow="120" yWindow="0" windowWidth="28680" windowHeight="15480" tabRatio="599" activeTab="6" xr2:uid="{27070F80-89CF-4E15-8F14-835BDE193743}"/>
   </bookViews>
   <sheets>
     <sheet name="PVModules" sheetId="25" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="WindTurbines" sheetId="38" r:id="rId4"/>
     <sheet name="FX-20kW" sheetId="39" r:id="rId5"/>
     <sheet name="TUGE-10kW" sheetId="41" r:id="rId6"/>
+    <sheet name="Boilers" sheetId="42" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
   <si>
     <t>Voc_STC</t>
   </si>
@@ -209,6 +210,24 @@
   </si>
   <si>
     <t>TUGE-10kW</t>
+  </si>
+  <si>
+    <t>Vitodens 050-W</t>
+  </si>
+  <si>
+    <t>P_out</t>
+  </si>
+  <si>
+    <t>fuel</t>
+  </si>
+  <si>
+    <t>Natural gas, LPG</t>
+  </si>
+  <si>
+    <t>P_min</t>
+  </si>
+  <si>
+    <t>C_OM_kWh</t>
   </si>
 </sst>
 </file>
@@ -267,9 +286,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -307,7 +326,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -413,7 +432,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -555,7 +574,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1577,7 +1596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0EA1E95-5149-4499-B4D9-6A20C5BF854C}">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1866,4 +1885,86 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AF105AB-C0E0-4CD7-A4BC-B72E3552AF70}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7">
+        <v>1.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Incorporación de CHPs en el modelo y energía térmica no suministrada
</commit_message>
<xml_diff>
--- a/Catalogo.xlsx
+++ b/Catalogo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Documents\GitHub\Tesis_Maestria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B77AB4-379A-4730-BCF4-F5DAD1C0CCB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD1795A-925C-4526-B26A-FC3BCD7113CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="0" windowWidth="28680" windowHeight="15480" tabRatio="599" activeTab="6" xr2:uid="{27070F80-89CF-4E15-8F14-835BDE193743}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="599" firstSheet="4" activeTab="7" xr2:uid="{27070F80-89CF-4E15-8F14-835BDE193743}"/>
   </bookViews>
   <sheets>
     <sheet name="PVModules" sheetId="25" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="FX-20kW" sheetId="39" r:id="rId5"/>
     <sheet name="TUGE-10kW" sheetId="41" r:id="rId6"/>
     <sheet name="Boilers" sheetId="42" r:id="rId7"/>
+    <sheet name="CHPs" sheetId="43" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="74">
   <si>
     <t>Voc_STC</t>
   </si>
@@ -215,19 +216,52 @@
     <t>Vitodens 050-W</t>
   </si>
   <si>
-    <t>P_out</t>
-  </si>
-  <si>
     <t>fuel</t>
   </si>
   <si>
     <t>Natural gas, LPG</t>
   </si>
   <si>
-    <t>P_min</t>
-  </si>
-  <si>
     <t>C_OM_kWh</t>
+  </si>
+  <si>
+    <t>P_min_porc</t>
+  </si>
+  <si>
+    <t>y_n</t>
+  </si>
+  <si>
+    <t>lamd_n</t>
+  </si>
+  <si>
+    <t>P_th_nom</t>
+  </si>
+  <si>
+    <t>Vitodens 020-W</t>
+  </si>
+  <si>
+    <t>Type 1 - 10kW</t>
+  </si>
+  <si>
+    <t>Type 2 - 20kW</t>
+  </si>
+  <si>
+    <t>n_nom_th</t>
+  </si>
+  <si>
+    <t>n_nom_el</t>
+  </si>
+  <si>
+    <t>y_n_el</t>
+  </si>
+  <si>
+    <t>lamd_n_el</t>
+  </si>
+  <si>
+    <t>y_n_th</t>
+  </si>
+  <si>
+    <t>lamd_n_th</t>
   </si>
 </sst>
 </file>
@@ -1889,79 +1923,266 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AF105AB-C0E0-4CD7-A4BC-B72E3552AF70}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>58</v>
       </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>312</v>
+      </c>
+      <c r="C5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="C6">
+        <v>1.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8">
+        <v>0.45760000000000001</v>
+      </c>
+      <c r="C8">
+        <v>0.45760000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9">
+        <v>0.65990000000000004</v>
+      </c>
+      <c r="C9">
+        <v>0.65990000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C318973-D1B9-4A7B-AA66-C06379304896}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
       <c r="B2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8000</v>
+      </c>
+      <c r="C2">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>61</v>
       </c>
-      <c r="B3">
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
       <c r="B4">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="C4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="B5">
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B7">
-        <v>1.2999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="C7">
+        <v>0.48599999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="C8">
+        <v>0.41699999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9">
+        <v>0.25480000000000003</v>
+      </c>
+      <c r="C9">
+        <v>0.26490000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10">
+        <v>2.2134999999999998</v>
+      </c>
+      <c r="C10">
+        <v>2.2229999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11">
+        <v>0.22439999999999999</v>
+      </c>
+      <c r="C11">
+        <v>0.23549999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12">
+        <v>0.95450000000000002</v>
+      </c>
+      <c r="C12">
+        <v>0.96550000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modelo multi energético versión 1
</commit_message>
<xml_diff>
--- a/Catalogo.xlsx
+++ b/Catalogo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Documents\GitHub\Tesis_Maestria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD1795A-925C-4526-B26A-FC3BCD7113CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACCA1630-6346-4B5A-8DC9-EF19617F0681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="599" firstSheet="4" activeTab="7" xr2:uid="{27070F80-89CF-4E15-8F14-835BDE193743}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="599" firstSheet="1" activeTab="9" xr2:uid="{27070F80-89CF-4E15-8F14-835BDE193743}"/>
   </bookViews>
   <sheets>
     <sheet name="PVModules" sheetId="25" r:id="rId1"/>
@@ -21,6 +21,8 @@
     <sheet name="TUGE-10kW" sheetId="41" r:id="rId6"/>
     <sheet name="Boilers" sheetId="42" r:id="rId7"/>
     <sheet name="CHPs" sheetId="43" r:id="rId8"/>
+    <sheet name="AbsorptionChillers" sheetId="44" r:id="rId9"/>
+    <sheet name="ElectricChillers" sheetId="45" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="78">
   <si>
     <t>Voc_STC</t>
   </si>
@@ -213,9 +215,6 @@
     <t>TUGE-10kW</t>
   </si>
   <si>
-    <t>Vitodens 050-W</t>
-  </si>
-  <si>
     <t>fuel</t>
   </si>
   <si>
@@ -237,15 +236,6 @@
     <t>P_th_nom</t>
   </si>
   <si>
-    <t>Vitodens 020-W</t>
-  </si>
-  <si>
-    <t>Type 1 - 10kW</t>
-  </si>
-  <si>
-    <t>Type 2 - 20kW</t>
-  </si>
-  <si>
     <t>n_nom_th</t>
   </si>
   <si>
@@ -262,6 +252,30 @@
   </si>
   <si>
     <t>lamd_n_th</t>
+  </si>
+  <si>
+    <t>Type 1 - 5kW</t>
+  </si>
+  <si>
+    <t>Type 2 - 10kW</t>
+  </si>
+  <si>
+    <t>Type 1 - 5kWth</t>
+  </si>
+  <si>
+    <t>Type 1 - 10kWth</t>
+  </si>
+  <si>
+    <t>P_cl_nom</t>
+  </si>
+  <si>
+    <t>Type 1 - 5kWcl</t>
+  </si>
+  <si>
+    <t>Type 1 - 10kWcl</t>
+  </si>
+  <si>
+    <t>Type 1 - 8kWcl</t>
   </si>
 </sst>
 </file>
@@ -619,7 +633,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C17"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -816,6 +830,113 @@
       </c>
       <c r="C17" s="2">
         <v>1.1299999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F424A40-ACCC-4017-8013-4BE203A582B6}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>1016</v>
+      </c>
+      <c r="C2">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5">
+        <v>2E-3</v>
+      </c>
+      <c r="C5">
+        <v>1.8E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7">
+        <v>4.3499999999999997E-2</v>
+      </c>
+      <c r="C7">
+        <v>4.4600000000000001E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8">
+        <v>0.11890000000000001</v>
+      </c>
+      <c r="C8">
+        <v>0.13869999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1926,7 +2047,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A4" sqref="A4:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1940,37 +2061,37 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
         <v>58</v>
       </c>
-      <c r="B2" t="s">
-        <v>59</v>
-      </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>32</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4">
         <v>0.2</v>
@@ -1984,15 +2105,15 @@
         <v>20</v>
       </c>
       <c r="B5">
-        <v>312</v>
+        <v>78</v>
       </c>
       <c r="C5">
-        <v>500</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6">
         <v>1.2999999999999999E-2</v>
@@ -2014,7 +2135,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8">
         <v>0.45760000000000001</v>
@@ -2025,7 +2146,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9">
         <v>0.65990000000000004</v>
@@ -2043,8 +2164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C318973-D1B9-4A7B-AA66-C06379304896}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2058,10 +2179,10 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2069,10 +2190,10 @@
         <v>20</v>
       </c>
       <c r="B2">
-        <v>8000</v>
+        <v>4000</v>
       </c>
       <c r="C2">
-        <v>14000</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2080,15 +2201,15 @@
         <v>45</v>
       </c>
       <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
         <v>10</v>
-      </c>
-      <c r="C3">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4">
         <v>0.5</v>
@@ -2099,7 +2220,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5">
         <v>2.5000000000000001E-2</v>
@@ -2121,7 +2242,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B7">
         <v>0.47899999999999998</v>
@@ -2132,7 +2253,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B8">
         <v>0.40500000000000003</v>
@@ -2143,7 +2264,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B9">
         <v>0.25480000000000003</v>
@@ -2154,7 +2275,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B10">
         <v>2.2134999999999998</v>
@@ -2165,7 +2286,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B11">
         <v>0.22439999999999999</v>
@@ -2176,13 +2297,120 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B12">
         <v>0.95450000000000002</v>
       </c>
       <c r="C12">
         <v>0.96550000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{462C8D84-F137-49A2-9F6C-907BFF281104}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>865</v>
+      </c>
+      <c r="C2">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5">
+        <v>1.5E-3</v>
+      </c>
+      <c r="C5">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="C7">
+        <v>5.5E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8">
+        <v>1.3565</v>
+      </c>
+      <c r="C8">
+        <v>1.367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Primera ejecución con Cumaribo
</commit_message>
<xml_diff>
--- a/Catalogo.xlsx
+++ b/Catalogo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Documents\GitHub\Tesis_Maestria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8554378D-E82C-49FC-A286-73ED2B94EA02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5E5607-BB6E-4EE0-A7FF-3E3569688E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="599" firstSheet="3" activeTab="11" xr2:uid="{27070F80-89CF-4E15-8F14-835BDE193743}"/>
+    <workbookView xWindow="-240" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="599" firstSheet="3" activeTab="11" xr2:uid="{27070F80-89CF-4E15-8F14-835BDE193743}"/>
   </bookViews>
   <sheets>
     <sheet name="PVModules" sheetId="25" r:id="rId1"/>
@@ -295,10 +295,10 @@
     <t>U_loss</t>
   </si>
   <si>
-    <t>lamda_alpha</t>
-  </si>
-  <si>
     <t>Type 1 -2.8m2</t>
+  </si>
+  <si>
+    <t>lambda_alpha</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1067,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,7 +1081,7 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1105,7 +1105,7 @@
         <v>21</v>
       </c>
       <c r="B4">
-        <v>2.8</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1113,7 +1113,7 @@
         <v>80</v>
       </c>
       <c r="B5">
-        <v>0.85</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1121,12 +1121,12 @@
         <v>81</v>
       </c>
       <c r="B6">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B7">
         <v>0.75</v>
@@ -1142,7 +1142,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,7 +1317,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1402,7 +1402,7 @@
         <v>14</v>
       </c>
       <c r="B10">
-        <v>25</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Cambios 12 de marzo
</commit_message>
<xml_diff>
--- a/Catalogo.xlsx
+++ b/Catalogo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Documents\GitHub\Tesis_Maestria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D6037E-5BC5-4F14-AA04-84691E764010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A5AFD2-E7DD-437C-83B2-E57E3E7C604E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="599" activeTab="8" xr2:uid="{27070F80-89CF-4E15-8F14-835BDE193743}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="599" firstSheet="4" activeTab="6" xr2:uid="{27070F80-89CF-4E15-8F14-835BDE193743}"/>
   </bookViews>
   <sheets>
     <sheet name="PVModules" sheetId="25" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="81">
   <si>
     <t>Voc_STC</t>
   </si>
@@ -210,12 +210,6 @@
     <t>TUGE-10kW</t>
   </si>
   <si>
-    <t>fuel</t>
-  </si>
-  <si>
-    <t>Natural gas, LPG</t>
-  </si>
-  <si>
     <t>C_OM_kWh</t>
   </si>
   <si>
@@ -243,12 +237,6 @@
     <t>lamd_n_th</t>
   </si>
   <si>
-    <t>Type 1 - 5kWth</t>
-  </si>
-  <si>
-    <t>Type 1 - 10kWth</t>
-  </si>
-  <si>
     <t>P_cl_nom</t>
   </si>
   <si>
@@ -273,28 +261,34 @@
     <t>VacuumTube Elite 300</t>
   </si>
   <si>
-    <t>CompactHeat 500</t>
-  </si>
-  <si>
-    <t>PowerHeat 3000</t>
-  </si>
-  <si>
-    <t>CoolCompact 10</t>
-  </si>
-  <si>
-    <t>PowerCool 50</t>
-  </si>
-  <si>
-    <t>Compacto 1 etapas - 20 kW</t>
-  </si>
-  <si>
-    <t>Compacto 2 etapas - 30 kW</t>
-  </si>
-  <si>
-    <t>Microturbina de Gas</t>
-  </si>
-  <si>
-    <t>Motor Reciprocante de Gas Natural</t>
+    <t>Atmosférica Convencional - 40</t>
+  </si>
+  <si>
+    <t>Condensación - 35</t>
+  </si>
+  <si>
+    <t>Motor Reciprocante - 200</t>
+  </si>
+  <si>
+    <t>Microturbina - 65</t>
+  </si>
+  <si>
+    <t>CoolCompact 50</t>
+  </si>
+  <si>
+    <t>PowerCool 150</t>
+  </si>
+  <si>
+    <t>CompactHeat 20</t>
+  </si>
+  <si>
+    <t>Simple efecto - 50</t>
+  </si>
+  <si>
+    <t>Doble efecto - 100</t>
+  </si>
+  <si>
+    <t>PowerHeat 50</t>
   </si>
 </sst>
 </file>
@@ -808,7 +802,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,10 +816,10 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -833,43 +827,43 @@
         <v>20</v>
       </c>
       <c r="B2">
-        <v>2000</v>
+        <v>15000</v>
       </c>
       <c r="C2">
-        <v>7500</v>
+        <v>32000</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C3">
-        <v>50</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B4">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
         <v>0.25</v>
-      </c>
-      <c r="C4">
-        <v>0.2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5">
-        <v>0.01</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="C5">
-        <v>8.0000000000000002E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -885,24 +879,24 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B7">
-        <v>0.8</v>
+        <v>3.2</v>
       </c>
       <c r="C7">
-        <v>0.85</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B8">
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
       <c r="C8">
-        <v>0.05</v>
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>
@@ -915,7 +909,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,10 +923,10 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -940,10 +934,10 @@
         <v>20</v>
       </c>
       <c r="B2">
-        <v>250</v>
+        <v>1500</v>
       </c>
       <c r="C2">
-        <v>1200</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -951,18 +945,18 @@
         <v>45</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C3">
-        <v>30</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B4">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="C4">
         <v>0.1</v>
@@ -970,7 +964,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5">
         <v>0.01</v>
@@ -987,7 +981,7 @@
         <v>15</v>
       </c>
       <c r="C6">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1026,10 +1020,10 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1067,7 +1061,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B5">
         <v>0.92</v>
@@ -1078,7 +1072,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B6">
         <v>6</v>
@@ -1089,7 +1083,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B7">
         <v>0.9</v>
@@ -1133,10 +1127,10 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2213,16 +2207,16 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AF105AB-C0E0-4CD7-A4BC-B72E3552AF70}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2230,97 +2224,86 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" t="s">
-        <v>55</v>
+        <v>58</v>
+      </c>
+      <c r="B2">
+        <v>35</v>
+      </c>
+      <c r="C2">
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="C3">
-        <v>50</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B4">
-        <v>0.15</v>
+        <v>6500</v>
       </c>
       <c r="C4">
-        <v>0.2</v>
+        <v>4800</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="B5">
-        <v>5000</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="C5">
-        <v>8000</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="B6">
-        <v>0.02</v>
+        <v>20</v>
       </c>
       <c r="C6">
-        <v>1.4999999999999999E-2</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="B7">
-        <v>15</v>
+        <v>0.94</v>
       </c>
       <c r="C7">
-        <v>20</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8">
-        <v>0.92</v>
+        <v>0.06</v>
       </c>
       <c r="C8">
-        <v>0.88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9">
-        <v>0.08</v>
-      </c>
-      <c r="C9">
         <v>0.12</v>
       </c>
     </row>
@@ -2334,7 +2317,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2349,10 +2332,10 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2379,7 +2362,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B4">
         <v>0.3</v>
@@ -2390,7 +2373,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5">
         <v>1.4999999999999999E-2</v>
@@ -2412,46 +2395,46 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B7">
+        <v>0.3</v>
+      </c>
+      <c r="C7">
         <v>0.25</v>
-      </c>
-      <c r="C7">
-        <v>0.3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B8">
-        <v>0.75</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C8">
-        <v>0.65</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B9">
-        <v>0.4</v>
+        <v>0.18</v>
       </c>
       <c r="C9">
-        <v>0.45</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B10">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="C10">
-        <v>0.5</v>
+        <v>0.35</v>
       </c>
     </row>
   </sheetData>
@@ -2463,8 +2446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{462C8D84-F137-49A2-9F6C-907BFF281104}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2477,10 +2460,10 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
         <v>79</v>
-      </c>
-      <c r="C1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2488,26 +2471,26 @@
         <v>20</v>
       </c>
       <c r="B2">
-        <v>16000</v>
+        <v>25000</v>
       </c>
       <c r="C2">
-        <v>23000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C3">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B4">
         <v>0.15</v>
@@ -2518,13 +2501,13 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="C5">
-        <v>2.5000000000000001E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2540,24 +2523,24 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B7">
-        <v>0.55000000000000004</v>
+        <v>0.6</v>
       </c>
       <c r="C7">
-        <v>0.65</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B8">
-        <v>0.35</v>
+        <v>0.2</v>
       </c>
       <c r="C8">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>